<commit_message>
DCM commit on 20230925
</commit_message>
<xml_diff>
--- a/03.設計/詳細設計書_STB03（DRAW）.xlsx
+++ b/03.設計/詳細設計書_STB03（DRAW）.xlsx
@@ -767,19 +767,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>視界エリア（黄色プレイヤー時）</t>
-    <rPh sb="0" eb="2">
-      <t>シカイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>キイロ</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>ジ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>21 ~ 25</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1129,6 +1116,19 @@
   </si>
   <si>
     <t>MT</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>視界エリア（黄プレイヤー時）</t>
+    <rPh sb="0" eb="2">
+      <t>シカイ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ジ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1782,6 +1782,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1791,29 +1815,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1833,15 +1848,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1859,15 +1868,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="G15" s="82"/>
       <c r="H15" s="83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I15" s="84"/>
       <c r="J15" s="84"/>
@@ -2442,58 +2442,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="94" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
       <c r="P1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="95" t="str">
+      <c r="Q1" s="89" t="str">
         <f>D5</f>
         <v>MT</v>
       </c>
-      <c r="R1" s="95"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A2" s="93"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
       <c r="P2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="96">
+      <c r="Q2" s="90">
         <f>B5</f>
         <v>45170</v>
       </c>
-      <c r="R2" s="95"/>
+      <c r="R2" s="89"/>
     </row>
     <row r="3" spans="1:18" ht="22.5" customHeight="1">
       <c r="A3" s="20"/>
@@ -2519,435 +2519,435 @@
       <c r="A4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97" t="s">
+      <c r="E4" s="91"/>
+      <c r="F4" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97" t="s">
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
     </row>
     <row r="5" spans="1:18" ht="22.5" customHeight="1">
       <c r="A5" s="22">
         <v>1</v>
       </c>
-      <c r="B5" s="90">
+      <c r="B5" s="92">
         <v>45170</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91" t="s">
+      <c r="C5" s="92"/>
+      <c r="D5" s="93" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="92" t="s">
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="92"/>
-      <c r="Q5" s="92"/>
-      <c r="R5" s="92"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="94"/>
     </row>
     <row r="6" spans="1:18" ht="22.5" customHeight="1">
       <c r="A6" s="23">
         <v>2</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="89"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="89"/>
-      <c r="O6" s="89"/>
-      <c r="P6" s="89"/>
-      <c r="Q6" s="89"/>
-      <c r="R6" s="89"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
+      <c r="P6" s="97"/>
+      <c r="Q6" s="97"/>
+      <c r="R6" s="97"/>
     </row>
     <row r="7" spans="1:18" ht="27" customHeight="1">
       <c r="A7" s="23">
         <v>3</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="89"/>
-      <c r="Q7" s="89"/>
-      <c r="R7" s="89"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="97"/>
+      <c r="R7" s="97"/>
     </row>
     <row r="8" spans="1:18" ht="27" customHeight="1">
       <c r="A8" s="23">
         <v>4</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="89"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="97"/>
+      <c r="Q8" s="97"/>
+      <c r="R8" s="97"/>
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1">
       <c r="A9" s="23">
         <v>5</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="87"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="89"/>
-      <c r="M9" s="89"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="89"/>
-      <c r="P9" s="89"/>
-      <c r="Q9" s="89"/>
-      <c r="R9" s="89"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="97"/>
+      <c r="R9" s="97"/>
     </row>
     <row r="10" spans="1:18" ht="27" customHeight="1">
       <c r="A10" s="23">
         <v>6</v>
       </c>
-      <c r="B10" s="87"/>
-      <c r="C10" s="87"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="89"/>
-      <c r="Q10" s="89"/>
-      <c r="R10" s="89"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
+      <c r="N10" s="97"/>
+      <c r="O10" s="97"/>
+      <c r="P10" s="97"/>
+      <c r="Q10" s="97"/>
+      <c r="R10" s="97"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1">
       <c r="A11" s="23">
         <v>7</v>
       </c>
-      <c r="B11" s="87"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="89"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="89"/>
-      <c r="O11" s="89"/>
-      <c r="P11" s="89"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="89"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="97"/>
+      <c r="N11" s="97"/>
+      <c r="O11" s="97"/>
+      <c r="P11" s="97"/>
+      <c r="Q11" s="97"/>
+      <c r="R11" s="97"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1">
       <c r="A12" s="23">
         <v>8</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="89"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="97"/>
+      <c r="J12" s="97"/>
+      <c r="K12" s="97"/>
+      <c r="L12" s="97"/>
+      <c r="M12" s="97"/>
+      <c r="N12" s="97"/>
+      <c r="O12" s="97"/>
+      <c r="P12" s="97"/>
+      <c r="Q12" s="97"/>
+      <c r="R12" s="97"/>
     </row>
     <row r="13" spans="1:18" ht="27" customHeight="1">
       <c r="A13" s="23">
         <v>9</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="89"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="97"/>
+      <c r="P13" s="97"/>
+      <c r="Q13" s="97"/>
+      <c r="R13" s="97"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1">
       <c r="A14" s="23">
         <v>10</v>
       </c>
-      <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="89"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="89"/>
-      <c r="R14" s="89"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="97"/>
+      <c r="N14" s="97"/>
+      <c r="O14" s="97"/>
+      <c r="P14" s="97"/>
+      <c r="Q14" s="97"/>
+      <c r="R14" s="97"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1">
       <c r="A15" s="23">
         <v>11</v>
       </c>
-      <c r="B15" s="87"/>
-      <c r="C15" s="87"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="89"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="97"/>
+      <c r="O15" s="97"/>
+      <c r="P15" s="97"/>
+      <c r="Q15" s="97"/>
+      <c r="R15" s="97"/>
     </row>
     <row r="16" spans="1:18" ht="27" customHeight="1">
       <c r="A16" s="23">
         <v>12</v>
       </c>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="89"/>
-      <c r="M16" s="89"/>
-      <c r="N16" s="89"/>
-      <c r="O16" s="89"/>
-      <c r="P16" s="89"/>
-      <c r="Q16" s="89"/>
-      <c r="R16" s="89"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="97"/>
+      <c r="O16" s="97"/>
+      <c r="P16" s="97"/>
+      <c r="Q16" s="97"/>
+      <c r="R16" s="97"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1">
       <c r="A17" s="23">
         <v>13</v>
       </c>
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="89"/>
-      <c r="M17" s="89"/>
-      <c r="N17" s="89"/>
-      <c r="O17" s="89"/>
-      <c r="P17" s="89"/>
-      <c r="Q17" s="89"/>
-      <c r="R17" s="89"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="97"/>
+      <c r="N17" s="97"/>
+      <c r="O17" s="97"/>
+      <c r="P17" s="97"/>
+      <c r="Q17" s="97"/>
+      <c r="R17" s="97"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1">
       <c r="A18" s="23">
         <v>14</v>
       </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="89"/>
-      <c r="K18" s="89"/>
-      <c r="L18" s="89"/>
-      <c r="M18" s="89"/>
-      <c r="N18" s="89"/>
-      <c r="O18" s="89"/>
-      <c r="P18" s="89"/>
-      <c r="Q18" s="89"/>
-      <c r="R18" s="89"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="97"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="97"/>
+      <c r="N18" s="97"/>
+      <c r="O18" s="97"/>
+      <c r="P18" s="97"/>
+      <c r="Q18" s="97"/>
+      <c r="R18" s="97"/>
     </row>
     <row r="19" spans="1:18" ht="27" customHeight="1">
       <c r="A19" s="23">
         <v>15</v>
       </c>
-      <c r="B19" s="87"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="89"/>
-      <c r="K19" s="89"/>
-      <c r="L19" s="89"/>
-      <c r="M19" s="89"/>
-      <c r="N19" s="89"/>
-      <c r="O19" s="89"/>
-      <c r="P19" s="89"/>
-      <c r="Q19" s="89"/>
-      <c r="R19" s="89"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="97"/>
+      <c r="N19" s="97"/>
+      <c r="O19" s="97"/>
+      <c r="P19" s="97"/>
+      <c r="Q19" s="97"/>
+      <c r="R19" s="97"/>
     </row>
     <row r="20" spans="1:18" ht="27" customHeight="1">
       <c r="A20" s="23">
         <v>16</v>
       </c>
-      <c r="B20" s="87"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="89"/>
-      <c r="K20" s="89"/>
-      <c r="L20" s="89"/>
-      <c r="M20" s="89"/>
-      <c r="N20" s="89"/>
-      <c r="O20" s="89"/>
-      <c r="P20" s="89"/>
-      <c r="Q20" s="89"/>
-      <c r="R20" s="89"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="97"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="97"/>
+      <c r="M20" s="97"/>
+      <c r="N20" s="97"/>
+      <c r="O20" s="97"/>
+      <c r="P20" s="97"/>
+      <c r="Q20" s="97"/>
+      <c r="R20" s="97"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1">
       <c r="A21" s="23">
         <v>17</v>
       </c>
-      <c r="B21" s="87"/>
-      <c r="C21" s="87"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="89"/>
-      <c r="J21" s="89"/>
-      <c r="K21" s="89"/>
-      <c r="L21" s="89"/>
-      <c r="M21" s="89"/>
-      <c r="N21" s="89"/>
-      <c r="O21" s="89"/>
-      <c r="P21" s="89"/>
-      <c r="Q21" s="89"/>
-      <c r="R21" s="89"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="96"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="97"/>
+      <c r="N21" s="97"/>
+      <c r="O21" s="97"/>
+      <c r="P21" s="97"/>
+      <c r="Q21" s="97"/>
+      <c r="R21" s="97"/>
     </row>
     <row r="22" spans="1:18" ht="27" customHeight="1">
       <c r="A22" s="23">
         <v>18</v>
       </c>
-      <c r="B22" s="87"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="89"/>
-      <c r="J22" s="89"/>
-      <c r="K22" s="89"/>
-      <c r="L22" s="89"/>
-      <c r="M22" s="89"/>
-      <c r="N22" s="89"/>
-      <c r="O22" s="89"/>
-      <c r="P22" s="89"/>
-      <c r="Q22" s="89"/>
-      <c r="R22" s="89"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="97"/>
+      <c r="J22" s="97"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="97"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="97"/>
+      <c r="Q22" s="97"/>
+      <c r="R22" s="97"/>
     </row>
     <row r="23" spans="1:18" ht="27" customHeight="1"/>
     <row r="24" spans="1:18" ht="27" customHeight="1"/>
@@ -2958,6 +2958,78 @@
     <row r="29" spans="1:18" ht="27" customHeight="1"/>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:R22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:R20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:R17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:R18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:R15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:R16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:R13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I14:R14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:R11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I12:R12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:R9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:R10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:R7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:R8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:R6"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D1:O2"/>
     <mergeCell ref="Q1:R1"/>
@@ -2966,78 +3038,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:R4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:R5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:R6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:R7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:R8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:R9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:R10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:R11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:R12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:R13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I14:R14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:R15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:R16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:R17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:R18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:R19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:R20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:R22"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.35433070866141736" footer="0.15748031496062992"/>
@@ -3067,112 +3067,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="104" t="s">
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="110" t="str">
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="113" t="str">
         <f>表紙!D6</f>
         <v>Street Biter (STB)</v>
       </c>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="104" t="s">
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="V1" s="114"/>
+      <c r="W1" s="114"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="106"/>
-      <c r="AA1" s="114" t="str">
+      <c r="Z1" s="102"/>
+      <c r="AA1" s="99" t="str">
         <f>更新履歴!D5</f>
         <v>MT</v>
       </c>
-      <c r="AB1" s="114"/>
-      <c r="AC1" s="114"/>
-      <c r="AD1" s="114"/>
-      <c r="AE1" s="114" t="s">
+      <c r="AB1" s="99"/>
+      <c r="AC1" s="99"/>
+      <c r="AD1" s="99"/>
+      <c r="AE1" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="AF1" s="114"/>
-      <c r="AG1" s="113" t="str">
+      <c r="AF1" s="99"/>
+      <c r="AG1" s="98" t="str">
         <f>VLOOKUP(MAX(更新履歴!B:B),更新履歴!B:D,3,FALSE)</f>
         <v>MT</v>
       </c>
-      <c r="AH1" s="114"/>
-      <c r="AI1" s="114"/>
-      <c r="AJ1" s="114"/>
+      <c r="AH1" s="99"/>
+      <c r="AI1" s="99"/>
+      <c r="AJ1" s="99"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="101"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104" t="s">
+      <c r="A2" s="106"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="107" t="str">
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="110" t="str">
         <f>RIGHT(表紙!D7,LEN(表紙!D7)-FIND("_",表紙!D7))</f>
         <v>03_DRAW</v>
       </c>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="108"/>
-      <c r="X2" s="109"/>
-      <c r="Y2" s="104" t="s">
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="112"/>
+      <c r="Y2" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="106"/>
-      <c r="AA2" s="115">
+      <c r="Z2" s="102"/>
+      <c r="AA2" s="100">
         <f>更新履歴!B5</f>
         <v>45170</v>
       </c>
-      <c r="AB2" s="115"/>
-      <c r="AC2" s="115"/>
-      <c r="AD2" s="115"/>
-      <c r="AE2" s="114" t="s">
+      <c r="AB2" s="100"/>
+      <c r="AC2" s="100"/>
+      <c r="AD2" s="100"/>
+      <c r="AE2" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="AF2" s="114"/>
-      <c r="AG2" s="115">
+      <c r="AF2" s="99"/>
+      <c r="AG2" s="100">
         <f>MAX(更新履歴!B:B)</f>
         <v>45170</v>
       </c>
-      <c r="AH2" s="115"/>
-      <c r="AI2" s="115"/>
-      <c r="AJ2" s="115"/>
+      <c r="AH2" s="100"/>
+      <c r="AI2" s="100"/>
+      <c r="AJ2" s="100"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
       <c r="A3" s="35"/>
@@ -3938,7 +3938,7 @@
         <v>83</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G32" s="17"/>
       <c r="AC32" s="27"/>
@@ -4305,7 +4305,7 @@
       <c r="I50" s="64"/>
       <c r="J50" s="64"/>
       <c r="K50" s="75" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="L50" s="64"/>
       <c r="M50" s="64"/>
@@ -4325,19 +4325,19 @@
       <c r="A51" s="57"/>
       <c r="B51" s="17"/>
       <c r="C51" s="66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51" s="67"/>
       <c r="E51" s="67"/>
       <c r="F51" s="67"/>
       <c r="G51" s="76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H51" s="67"/>
       <c r="I51" s="67"/>
       <c r="J51" s="67"/>
       <c r="K51" s="76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L51" s="67"/>
       <c r="M51" s="67"/>
@@ -4357,19 +4357,19 @@
       <c r="A52" s="57"/>
       <c r="B52" s="17"/>
       <c r="C52" s="66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D52" s="67"/>
       <c r="E52" s="67"/>
       <c r="F52" s="67"/>
       <c r="G52" s="76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H52" s="67"/>
       <c r="I52" s="67"/>
       <c r="J52" s="67"/>
       <c r="K52" s="76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L52" s="67"/>
       <c r="M52" s="67"/>
@@ -4403,7 +4403,7 @@
         <v>35</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G54" s="17"/>
       <c r="AC54" s="27"/>
@@ -4418,7 +4418,7 @@
     <row r="55" spans="1:36" ht="15" customHeight="1">
       <c r="A55" s="59"/>
       <c r="B55" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G55" s="17"/>
       <c r="AC55" s="27"/>
@@ -4448,7 +4448,7 @@
         <v>36</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G57" s="17"/>
       <c r="AC57" s="27"/>
@@ -4463,7 +4463,7 @@
     <row r="58" spans="1:36" ht="15" customHeight="1">
       <c r="A58" s="59"/>
       <c r="B58" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G58" s="17"/>
       <c r="AC58" s="27"/>
@@ -4478,7 +4478,7 @@
     <row r="59" spans="1:36" ht="15" customHeight="1">
       <c r="A59" s="59"/>
       <c r="B59" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G59" s="17"/>
       <c r="AC59" s="27"/>
@@ -4499,23 +4499,23 @@
       <c r="E60" s="63"/>
       <c r="F60" s="63"/>
       <c r="G60" s="75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H60" s="65"/>
       <c r="I60" s="75" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J60" s="65"/>
       <c r="K60" s="75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L60" s="65"/>
       <c r="M60" s="75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N60" s="65"/>
       <c r="O60" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P60" s="65"/>
       <c r="AC60" s="71"/>
@@ -4536,23 +4536,23 @@
       <c r="E61" s="67"/>
       <c r="F61" s="67"/>
       <c r="G61" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H61" s="61"/>
       <c r="I61" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J61" s="61"/>
       <c r="K61" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L61" s="61"/>
       <c r="M61" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N61" s="61"/>
       <c r="O61" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P61" s="61"/>
       <c r="AC61" s="71"/>
@@ -4567,29 +4567,29 @@
     <row r="62" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="B62" s="70"/>
       <c r="C62" s="66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D62" s="67"/>
       <c r="E62" s="67"/>
       <c r="F62" s="67"/>
       <c r="G62" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H62" s="61"/>
       <c r="I62" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J62" s="61"/>
       <c r="K62" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L62" s="61"/>
       <c r="M62" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N62" s="61"/>
       <c r="O62" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P62" s="61"/>
       <c r="AC62" s="71"/>
@@ -4604,29 +4604,29 @@
     <row r="63" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="B63" s="70"/>
       <c r="C63" s="66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D63" s="67"/>
       <c r="E63" s="67"/>
       <c r="F63" s="67"/>
       <c r="G63" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H63" s="61"/>
       <c r="I63" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J63" s="61"/>
       <c r="K63" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L63" s="61"/>
       <c r="M63" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N63" s="61"/>
       <c r="O63" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P63" s="61"/>
       <c r="AC63" s="71"/>
@@ -4641,29 +4641,29 @@
     <row r="64" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="B64" s="70"/>
       <c r="C64" s="66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D64" s="67"/>
       <c r="E64" s="67"/>
       <c r="F64" s="67"/>
       <c r="G64" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H64" s="61"/>
       <c r="I64" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J64" s="61"/>
       <c r="K64" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L64" s="61"/>
       <c r="M64" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N64" s="61"/>
       <c r="O64" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P64" s="61"/>
       <c r="AC64" s="71"/>
@@ -4678,29 +4678,29 @@
     <row r="65" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="B65" s="70"/>
       <c r="C65" s="66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D65" s="67"/>
       <c r="E65" s="67"/>
       <c r="F65" s="67"/>
       <c r="G65" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H65" s="61"/>
       <c r="I65" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J65" s="61"/>
       <c r="K65" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L65" s="61"/>
       <c r="M65" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N65" s="61"/>
       <c r="O65" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P65" s="61"/>
       <c r="AC65" s="71"/>
@@ -4716,29 +4716,29 @@
       <c r="A66" s="59"/>
       <c r="B66" s="17"/>
       <c r="C66" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D66" s="67"/>
       <c r="E66" s="67"/>
       <c r="F66" s="67"/>
       <c r="G66" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H66" s="61"/>
       <c r="I66" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J66" s="61"/>
       <c r="K66" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L66" s="61"/>
       <c r="M66" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N66" s="61"/>
       <c r="O66" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P66" s="61"/>
       <c r="AC66" s="27"/>
@@ -4768,7 +4768,7 @@
         <v>37</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G68" s="17"/>
       <c r="AC68" s="27"/>
@@ -4783,7 +4783,7 @@
     <row r="69" spans="1:36" ht="15" customHeight="1">
       <c r="A69" s="57"/>
       <c r="B69" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C69" s="44"/>
       <c r="D69" s="44"/>
@@ -4808,7 +4808,7 @@
     <row r="70" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A70" s="70"/>
       <c r="B70" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC70" s="71"/>
       <c r="AD70" s="72"/>
@@ -4828,7 +4828,7 @@
       <c r="E71" s="63"/>
       <c r="F71" s="63"/>
       <c r="G71" s="75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H71" s="64"/>
       <c r="I71" s="64"/>
@@ -4850,7 +4850,7 @@
       <c r="E72" s="67"/>
       <c r="F72" s="67"/>
       <c r="G72" s="76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H72" s="67"/>
       <c r="I72" s="67"/>
@@ -4867,13 +4867,13 @@
     <row r="73" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A73" s="70"/>
       <c r="C73" s="66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D73" s="67"/>
       <c r="E73" s="67"/>
       <c r="F73" s="67"/>
       <c r="G73" s="76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H73" s="67"/>
       <c r="I73" s="67"/>
@@ -4891,13 +4891,13 @@
       <c r="A74" s="70"/>
       <c r="B74" s="78"/>
       <c r="C74" s="66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D74" s="67"/>
       <c r="E74" s="67"/>
       <c r="F74" s="67"/>
       <c r="G74" s="76" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H74" s="67"/>
       <c r="I74" s="67"/>
@@ -4914,13 +4914,13 @@
     <row r="75" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A75" s="74"/>
       <c r="C75" s="66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D75" s="67"/>
       <c r="E75" s="67"/>
       <c r="F75" s="67"/>
       <c r="G75" s="76" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H75" s="67"/>
       <c r="I75" s="67"/>
@@ -4942,7 +4942,7 @@
       <c r="E76" s="67"/>
       <c r="F76" s="67"/>
       <c r="G76" s="76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H76" s="67"/>
       <c r="I76" s="67"/>
@@ -4959,7 +4959,7 @@
     <row r="77" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A77" s="70"/>
       <c r="B77" s="44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC77" s="71"/>
       <c r="AD77" s="72"/>
@@ -4973,7 +4973,7 @@
     <row r="78" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A78" s="70"/>
       <c r="B78" s="44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC78" s="71"/>
       <c r="AD78" s="72"/>
@@ -4993,7 +4993,7 @@
       <c r="E79" s="63"/>
       <c r="F79" s="63"/>
       <c r="G79" s="75" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H79" s="64"/>
       <c r="I79" s="64"/>
@@ -5013,13 +5013,13 @@
     <row r="80" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A80" s="70"/>
       <c r="C80" s="66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D80" s="67"/>
       <c r="E80" s="67"/>
       <c r="F80" s="67"/>
       <c r="G80" s="76" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H80" s="67"/>
       <c r="I80" s="67"/>
@@ -5065,7 +5065,7 @@
     <row r="82" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A82" s="70"/>
       <c r="C82" s="66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D82" s="67"/>
       <c r="E82" s="67"/>
@@ -5091,7 +5091,7 @@
     <row r="83" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A83" s="70"/>
       <c r="C83" s="66" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D83" s="67"/>
       <c r="E83" s="67"/>
@@ -5145,7 +5145,7 @@
         <v>38</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AC85" s="71"/>
       <c r="AD85" s="72"/>
@@ -5159,7 +5159,7 @@
     <row r="86" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A86" s="74"/>
       <c r="B86" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC86" s="71"/>
       <c r="AD86" s="72"/>
@@ -5221,6 +5221,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I2:X2"/>
+    <mergeCell ref="I1:X1"/>
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="AG2:AJ2"/>
     <mergeCell ref="AA1:AD1"/>
@@ -5229,11 +5234,6 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I2:X2"/>
-    <mergeCell ref="I1:X1"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.35433070866141736" footer="0.15748031496062992"/>

</xml_diff>